<commit_message>
all updates revisions and migration analysis
</commit_message>
<xml_diff>
--- a/tables/SpatialAutocor_04.10.22.xlsx
+++ b/tables/SpatialAutocor_04.10.22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vistor/Documents/Work/GitHub/PhD/blackgrouse-hunting/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCD7A86-54DD-914B-A7BC-8B5C49608B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38AED654-32D8-CC4F-931F-AB9D49FB7FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,20 @@
     <sheet name="SpatialAutocor" sheetId="1" r:id="rId1"/>
     <sheet name="ForR" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1728,8 +1741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>